<commit_message>
updated to new fm profile format
</commit_message>
<xml_diff>
--- a/ftest/data/fm23/worked_example_policy_calculation_locfac_catxol_reinsurance.xlsx
+++ b/ftest/data/fm23/worked_example_policy_calculation_locfac_catxol_reinsurance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{274DA7F4-3229-4ABE-B3C9-04A26A6910FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B9502424-6FD3-45A5-AA77-746CDD9B3603}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="124">
   <si>
     <t>Limit</t>
   </si>
@@ -176,21 +176,6 @@
     <t>calcrule_id</t>
   </si>
   <si>
-    <t>allocrule_id</t>
-  </si>
-  <si>
-    <t>ccy_id</t>
-  </si>
-  <si>
-    <t>deductible</t>
-  </si>
-  <si>
-    <t>limits</t>
-  </si>
-  <si>
-    <t>share_prop_of_lim</t>
-  </si>
-  <si>
     <t>Policy Details</t>
   </si>
   <si>
@@ -381,6 +366,33 @@
   </si>
   <si>
     <t>Reinsurance Inuring level 2 - Cat XL</t>
+  </si>
+  <si>
+    <t>profile_id</t>
+  </si>
+  <si>
+    <t>deductible_1</t>
+  </si>
+  <si>
+    <t>deductible_2</t>
+  </si>
+  <si>
+    <t>deductible_3</t>
+  </si>
+  <si>
+    <t>attachment_1</t>
+  </si>
+  <si>
+    <t>limit_1</t>
+  </si>
+  <si>
+    <t>share_1</t>
+  </si>
+  <si>
+    <t>share_2</t>
+  </si>
+  <si>
+    <t>share_3</t>
   </si>
 </sst>
 </file>
@@ -388,8 +400,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -634,9 +646,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -796,6 +808,48 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -817,49 +871,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1206,8 +1217,8 @@
   </sheetPr>
   <dimension ref="A1:U95"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A79" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61:E61"/>
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56:E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1233,7 +1244,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1241,7 +1252,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1252,7 +1263,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="53" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1284,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1292,7 +1303,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1316,7 +1327,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -1468,7 +1479,7 @@
     </row>
     <row r="22" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>21</v>
@@ -1510,14 +1521,14 @@
         <v>27</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="11"/>
     </row>
     <row r="23" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="27"/>
@@ -1588,31 +1599,31 @@
     </row>
     <row r="25" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="66">
+        <v>61</v>
+      </c>
+      <c r="C25" s="64">
         <v>100</v>
       </c>
-      <c r="D25" s="66"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="66">
+      <c r="D25" s="64"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="64">
         <v>100</v>
       </c>
-      <c r="G25" s="66"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="68">
+      <c r="G25" s="64"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="66">
         <v>100</v>
       </c>
-      <c r="J25" s="66"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="66">
+      <c r="J25" s="64"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="64">
         <v>100</v>
       </c>
-      <c r="M25" s="66"/>
-      <c r="N25" s="67"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="65"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="11"/>
@@ -1725,7 +1736,7 @@
     </row>
     <row r="30" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="15"/>
@@ -1749,7 +1760,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C31" s="16">
         <f t="shared" ref="C31:N31" si="0">C28*C24</f>
@@ -1848,70 +1859,70 @@
     </row>
     <row r="34" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="69">
+        <v>63</v>
+      </c>
+      <c r="C34" s="67">
         <f>SUMIF($C$21:$N$21,C21,$C$31:$N$31)</f>
         <v>1600</v>
       </c>
-      <c r="D34" s="69"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="69">
+      <c r="D34" s="67"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="67">
         <f>SUMIF($C$21:$N$21,F21,$C$31:$N$31)</f>
         <v>1600</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="69">
+      <c r="G34" s="67"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="67">
         <f>SUMIF($C$21:$N$21,I21,$C$31:$N$31)</f>
         <v>1600</v>
       </c>
-      <c r="J34" s="69"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="69">
+      <c r="J34" s="67"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="67">
         <f>SUMIF($C$21:$N$21,L21,$C$31:$N$31)</f>
         <v>1600</v>
       </c>
-      <c r="M34" s="69"/>
-      <c r="N34" s="70"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="68"/>
       <c r="O34" s="8"/>
       <c r="P34" s="24"/>
       <c r="Q34" s="11"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="37" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="62">
+        <v>65</v>
+      </c>
+      <c r="C35" s="60">
         <f>MIN(C34, C25)</f>
         <v>100</v>
       </c>
-      <c r="D35" s="63"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="62">
+      <c r="D35" s="61"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="60">
         <f>MIN(F34, F25)</f>
         <v>100</v>
       </c>
-      <c r="G35" s="63"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="62">
+      <c r="G35" s="61"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="60">
         <f>MIN(I34, I25)</f>
         <v>100</v>
       </c>
-      <c r="J35" s="63"/>
-      <c r="K35" s="64"/>
-      <c r="L35" s="65">
+      <c r="J35" s="61"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="63">
         <f>MIN(L34, L25)</f>
         <v>100</v>
       </c>
-      <c r="M35" s="63"/>
-      <c r="N35" s="64"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="62"/>
       <c r="O35" s="12">
         <f>SUM(C35:N35)</f>
         <v>400</v>
@@ -1924,7 +1935,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C36" s="9">
         <f>C35*C$31/SUMIF($C$21:$N$21,C$21,$C$31:$N$31)</f>
@@ -2108,10 +2119,10 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C45" s="9">
         <f>SUMIF($C$20:$N$20,C20,$C$35:$N$35)</f>
@@ -2126,10 +2137,10 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C46" s="39">
         <f>MIN(C40, C45)*C41</f>
@@ -2144,10 +2155,10 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H47" s="41"/>
       <c r="N47" s="41"/>
@@ -2169,10 +2180,10 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C50" s="9">
         <f>$C$46*C$36/SUM($C$36:$H$36)</f>
@@ -2234,67 +2245,67 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C52" s="44" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="55">
-        <v>1</v>
-      </c>
-      <c r="D53" s="55"/>
-      <c r="E53" s="56"/>
+        <v>76</v>
+      </c>
+      <c r="C53" s="69">
+        <v>1</v>
+      </c>
+      <c r="D53" s="69"/>
+      <c r="E53" s="70"/>
       <c r="H53" s="41"/>
       <c r="N53" s="41"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="D54" s="55"/>
-      <c r="E54" s="56"/>
+        <v>77</v>
+      </c>
+      <c r="C54" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="69"/>
+      <c r="E54" s="70"/>
       <c r="H54" s="41"/>
       <c r="N54" s="41"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" s="55">
-        <v>1</v>
-      </c>
-      <c r="D55" s="55"/>
-      <c r="E55" s="56"/>
+        <v>78</v>
+      </c>
+      <c r="C55" s="69">
+        <v>1</v>
+      </c>
+      <c r="D55" s="69"/>
+      <c r="E55" s="70"/>
       <c r="H55" s="41"/>
       <c r="N55" s="41"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="59">
+        <v>79</v>
+      </c>
+      <c r="C56" s="73">
         <v>10</v>
       </c>
-      <c r="D56" s="59"/>
-      <c r="E56" s="56"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="70"/>
       <c r="H56" s="41"/>
       <c r="N56" s="41"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="C57" s="59">
+        <v>80</v>
+      </c>
+      <c r="C57" s="73">
         <f>MAX(0, SUM(C50:E50)-C56)</f>
         <v>90</v>
       </c>
-      <c r="D57" s="59"/>
-      <c r="E57" s="56"/>
+      <c r="D57" s="73"/>
+      <c r="E57" s="70"/>
       <c r="H57" s="41"/>
       <c r="N57" s="41"/>
     </row>
@@ -2302,49 +2313,49 @@
       <c r="A58" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="59">
+      <c r="C58" s="73">
         <v>100</v>
       </c>
-      <c r="D58" s="59"/>
-      <c r="E58" s="56"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="70"/>
       <c r="H58" s="41"/>
       <c r="N58" s="41"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C59" s="59">
+        <v>81</v>
+      </c>
+      <c r="C59" s="73">
         <f>IF(C58="Unlimited", C57, MIN(C57, C58))</f>
         <v>90</v>
       </c>
-      <c r="D59" s="59"/>
-      <c r="E59" s="56"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="70"/>
       <c r="H59" s="41"/>
       <c r="N59" s="41"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="C60" s="60">
+        <v>87</v>
+      </c>
+      <c r="C60" s="74">
         <v>0.5</v>
       </c>
-      <c r="D60" s="60"/>
-      <c r="E60" s="61"/>
+      <c r="D60" s="74"/>
+      <c r="E60" s="75"/>
       <c r="H60" s="41"/>
       <c r="N60" s="41"/>
     </row>
     <row r="61" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="59">
+        <v>88</v>
+      </c>
+      <c r="C61" s="73">
         <f>C60*C59</f>
         <v>45</v>
       </c>
-      <c r="D61" s="59"/>
-      <c r="E61" s="56"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="70"/>
       <c r="H61" s="41"/>
       <c r="N61" s="41"/>
     </row>
@@ -2352,38 +2363,38 @@
       <c r="A62" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="58"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="72"/>
       <c r="H62" s="41"/>
       <c r="N62" s="41"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" s="57"/>
-      <c r="D63" s="57"/>
-      <c r="E63" s="58"/>
+        <v>82</v>
+      </c>
+      <c r="C63" s="71"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="72"/>
       <c r="H63" s="41"/>
       <c r="N63" s="41"/>
     </row>
     <row r="64" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" s="59">
+        <v>83</v>
+      </c>
+      <c r="C64" s="73">
         <f>MIN(C61,IF(OR(C63="Unlimited",C63=""),10^18,C63))</f>
         <v>45</v>
       </c>
-      <c r="D64" s="59"/>
-      <c r="E64" s="56"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="70"/>
       <c r="H64" s="41"/>
       <c r="N64" s="41"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="48" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C65" s="13">
         <f>((SUM($C$50:$E$50)-$C$64)*C$50/SUM($C$50:$E$50))</f>
@@ -2440,12 +2451,12 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B66" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="N67" s="41"/>
       <c r="O67" s="2">
@@ -2454,16 +2465,16 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="45" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="N68" s="41"/>
       <c r="O68" s="53" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="45" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="N69" s="41"/>
       <c r="O69" s="2">
@@ -2472,7 +2483,7 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="45" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N70" s="41"/>
       <c r="O70" s="2">
@@ -2481,7 +2492,7 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="46" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N71" s="41"/>
       <c r="O71" s="6">
@@ -2503,7 +2514,7 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="46" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N73" s="41"/>
       <c r="O73" s="6">
@@ -2515,7 +2526,7 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="45" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="N74" s="41"/>
       <c r="O74" s="51">
@@ -2525,7 +2536,7 @@
     </row>
     <row r="75" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="46" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N75" s="41"/>
       <c r="O75" s="2">
@@ -2541,13 +2552,13 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="45" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="N77" s="41"/>
     </row>
     <row r="78" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="47" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="N78" s="41"/>
       <c r="O78" s="6">
@@ -2559,53 +2570,53 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="C79" s="71">
+        <v>93</v>
+      </c>
+      <c r="C79" s="55">
         <f>$O$78*C$65/$O$65</f>
         <v>7.746478873239437</v>
       </c>
-      <c r="D79" s="71">
+      <c r="D79" s="55">
         <f t="shared" ref="D79:N79" si="10">$O$78*D$65/$O$65</f>
         <v>3.8732394366197185</v>
       </c>
-      <c r="E79" s="71">
+      <c r="E79" s="55">
         <f t="shared" si="10"/>
         <v>3.8732394366197185</v>
       </c>
-      <c r="F79" s="71">
+      <c r="F79" s="55">
         <f t="shared" si="10"/>
         <v>14.084507042253522</v>
       </c>
-      <c r="G79" s="71">
+      <c r="G79" s="55">
         <f t="shared" si="10"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="H79" s="71">
+      <c r="H79" s="55">
         <f t="shared" si="10"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="I79" s="71">
+      <c r="I79" s="55">
         <f t="shared" si="10"/>
         <v>14.084507042253522</v>
       </c>
-      <c r="J79" s="71">
+      <c r="J79" s="55">
         <f t="shared" si="10"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="K79" s="71">
+      <c r="K79" s="55">
         <f t="shared" si="10"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="L79" s="71">
+      <c r="L79" s="55">
         <f t="shared" si="10"/>
         <v>14.084507042253522</v>
       </c>
-      <c r="M79" s="71">
+      <c r="M79" s="55">
         <f t="shared" si="10"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="N79" s="72">
+      <c r="N79" s="56">
         <f t="shared" si="10"/>
         <v>7.042253521126761</v>
       </c>
@@ -2616,12 +2627,12 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B81" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="45" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="N82" s="41"/>
       <c r="O82" s="2">
@@ -2630,16 +2641,16 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="45" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="N83" s="41"/>
       <c r="O83" s="53" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="45" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="N84" s="41"/>
       <c r="O84" s="2">
@@ -2648,7 +2659,7 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="45" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N85" s="41"/>
       <c r="O85" s="6">
@@ -2657,7 +2668,7 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="46" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N86" s="41"/>
       <c r="O86" s="6">
@@ -2676,7 +2687,7 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="46" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N88" s="41"/>
       <c r="O88" s="6">
@@ -2686,7 +2697,7 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="45" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="N89" s="41"/>
       <c r="O89" s="51">
@@ -2695,7 +2706,7 @@
     </row>
     <row r="90" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="46" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N90" s="41"/>
     </row>
@@ -2707,13 +2718,13 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="45" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="N92" s="41"/>
     </row>
     <row r="93" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="47" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="N93" s="41"/>
       <c r="O93" s="6">
@@ -2723,53 +2734,53 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="C94" s="71">
+        <v>94</v>
+      </c>
+      <c r="C94" s="55">
         <f>$O$93*C$65/$O$65</f>
         <v>7.746478873239437</v>
       </c>
-      <c r="D94" s="71">
+      <c r="D94" s="55">
         <f t="shared" ref="D94:N94" si="11">$O$93*D$65/$O$65</f>
         <v>3.8732394366197185</v>
       </c>
-      <c r="E94" s="71">
+      <c r="E94" s="55">
         <f t="shared" si="11"/>
         <v>3.8732394366197185</v>
       </c>
-      <c r="F94" s="71">
+      <c r="F94" s="55">
         <f t="shared" si="11"/>
         <v>14.084507042253522</v>
       </c>
-      <c r="G94" s="71">
+      <c r="G94" s="55">
         <f t="shared" si="11"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="H94" s="71">
+      <c r="H94" s="55">
         <f t="shared" si="11"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="I94" s="71">
+      <c r="I94" s="55">
         <f t="shared" si="11"/>
         <v>14.084507042253522</v>
       </c>
-      <c r="J94" s="71">
+      <c r="J94" s="55">
         <f t="shared" si="11"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="K94" s="71">
+      <c r="K94" s="55">
         <f t="shared" si="11"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="L94" s="71">
+      <c r="L94" s="55">
         <f t="shared" si="11"/>
         <v>14.084507042253522</v>
       </c>
-      <c r="M94" s="71">
+      <c r="M94" s="55">
         <f t="shared" si="11"/>
         <v>7.042253521126761</v>
       </c>
-      <c r="N94" s="72">
+      <c r="N94" s="56">
         <f t="shared" si="11"/>
         <v>7.042253521126761</v>
       </c>
@@ -2780,53 +2791,53 @@
     </row>
     <row r="95" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="C95" s="73">
+        <v>90</v>
+      </c>
+      <c r="C95" s="57">
         <f>C65-C79-C94</f>
         <v>12.007042253521128</v>
       </c>
-      <c r="D95" s="73">
+      <c r="D95" s="57">
         <f t="shared" ref="D95:N95" si="12">D65-D79-D94</f>
         <v>6.0035211267605639</v>
       </c>
-      <c r="E95" s="73">
+      <c r="E95" s="57">
         <f t="shared" si="12"/>
         <v>6.0035211267605639</v>
       </c>
-      <c r="F95" s="73">
+      <c r="F95" s="57">
         <f t="shared" si="12"/>
         <v>21.83098591549296</v>
       </c>
-      <c r="G95" s="73">
+      <c r="G95" s="57">
         <f t="shared" si="12"/>
         <v>10.91549295774648</v>
       </c>
-      <c r="H95" s="73">
+      <c r="H95" s="57">
         <f t="shared" si="12"/>
         <v>10.91549295774648</v>
       </c>
-      <c r="I95" s="73">
+      <c r="I95" s="57">
         <f t="shared" si="12"/>
         <v>21.83098591549296</v>
       </c>
-      <c r="J95" s="73">
+      <c r="J95" s="57">
         <f t="shared" si="12"/>
         <v>10.91549295774648</v>
       </c>
-      <c r="K95" s="73">
+      <c r="K95" s="57">
         <f t="shared" si="12"/>
         <v>10.91549295774648</v>
       </c>
-      <c r="L95" s="73">
+      <c r="L95" s="57">
         <f t="shared" si="12"/>
         <v>21.83098591549296</v>
       </c>
-      <c r="M95" s="73">
+      <c r="M95" s="57">
         <f t="shared" si="12"/>
         <v>10.91549295774648</v>
       </c>
-      <c r="N95" s="74">
+      <c r="N95" s="58">
         <f t="shared" si="12"/>
         <v>10.91549295774648</v>
       </c>
@@ -2837,6 +2848,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="I35:K35"/>
@@ -2849,18 +2872,6 @@
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="L34:N34"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -2876,10 +2887,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U74"/>
+  <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2901,18 +2912,18 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -2941,13 +2952,13 @@
         <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" t="s">
         <v>106</v>
-      </c>
-      <c r="M4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2975,11 +2986,11 @@
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" s="75">
+      <c r="K5" s="59">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -3010,11 +3021,11 @@
       <c r="J6">
         <v>2</v>
       </c>
-      <c r="K6" s="75">
+      <c r="K6" s="59">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -3045,11 +3056,11 @@
       <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7" s="75">
+      <c r="K7" s="59">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -3080,11 +3091,11 @@
       <c r="J8">
         <v>4</v>
       </c>
-      <c r="K8" s="75">
+      <c r="K8" s="59">
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -3115,11 +3126,11 @@
       <c r="J9">
         <v>5</v>
       </c>
-      <c r="K9" s="75">
+      <c r="K9" s="59">
         <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -3150,11 +3161,11 @@
       <c r="J10">
         <v>6</v>
       </c>
-      <c r="K10" s="75">
+      <c r="K10" s="59">
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -3185,11 +3196,11 @@
       <c r="J11">
         <v>7</v>
       </c>
-      <c r="K11" s="75">
+      <c r="K11" s="59">
         <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M11">
         <v>2</v>
@@ -3220,11 +3231,11 @@
       <c r="J12">
         <v>8</v>
       </c>
-      <c r="K12" s="75">
+      <c r="K12" s="59">
         <v>3</v>
       </c>
       <c r="L12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="M12">
         <v>2</v>
@@ -3255,11 +3266,11 @@
       <c r="J13">
         <v>9</v>
       </c>
-      <c r="K13" s="75">
+      <c r="K13" s="59">
         <v>3</v>
       </c>
       <c r="L13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="M13">
         <v>2</v>
@@ -3290,11 +3301,11 @@
       <c r="J14">
         <v>10</v>
       </c>
-      <c r="K14" s="75">
+      <c r="K14" s="59">
         <v>4</v>
       </c>
       <c r="L14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M14">
         <v>2</v>
@@ -3325,11 +3336,11 @@
       <c r="J15">
         <v>11</v>
       </c>
-      <c r="K15" s="75">
+      <c r="K15" s="59">
         <v>4</v>
       </c>
       <c r="L15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="M15">
         <v>2</v>
@@ -3360,36 +3371,36 @@
       <c r="J16">
         <v>12</v>
       </c>
-      <c r="K16" s="75">
+      <c r="K16" s="59">
         <v>4</v>
       </c>
       <c r="L16" t="s">
+        <v>104</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" t="s">
         <v>109</v>
       </c>
-      <c r="M16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" t="s">
-        <v>114</v>
-      </c>
       <c r="J21" t="s">
-        <v>115</v>
-      </c>
-      <c r="S21" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="U21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -3412,37 +3423,46 @@
         <v>49</v>
       </c>
       <c r="J22" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="K22" t="s">
         <v>50</v>
       </c>
       <c r="L22" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="M22" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="N22" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="O22" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="P22" t="s">
-        <v>55</v>
+        <v>120</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>121</v>
+      </c>
+      <c r="R22" t="s">
+        <v>122</v>
       </c>
       <c r="S22" t="s">
-        <v>117</v>
-      </c>
-      <c r="T22" t="s">
+        <v>123</v>
+      </c>
+      <c r="U22" t="s">
+        <v>112</v>
+      </c>
+      <c r="V22" t="s">
         <v>48</v>
       </c>
-      <c r="U22" t="s">
+      <c r="W22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3471,31 +3491,40 @@
         <v>1</v>
       </c>
       <c r="L23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M23">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <v>10000</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
         <v>0</v>
       </c>
       <c r="S23">
-        <v>1</v>
-      </c>
-      <c r="T23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -3524,31 +3553,40 @@
         <v>1</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
         <v>100</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
         <v>0</v>
       </c>
       <c r="S24">
-        <v>2</v>
-      </c>
-      <c r="T24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="V24">
+        <v>2</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3577,31 +3615,40 @@
         <v>1</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
-      <c r="O25" s="43">
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
         <v>100</v>
       </c>
-      <c r="P25" s="43">
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
         <v>0</v>
       </c>
       <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="U25">
         <v>3</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <v>3</v>
       </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3630,31 +3677,40 @@
         <v>1</v>
       </c>
       <c r="L26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N26">
         <v>0</v>
       </c>
-      <c r="O26" s="43">
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
         <v>10000</v>
       </c>
-      <c r="P26" s="43">
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
         <v>0</v>
       </c>
       <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="U26">
         <v>4</v>
       </c>
-      <c r="T26">
+      <c r="V26">
         <v>4</v>
       </c>
-      <c r="U26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>5</v>
       </c>
@@ -3683,31 +3739,40 @@
         <v>1</v>
       </c>
       <c r="L27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N27">
         <v>0</v>
       </c>
-      <c r="O27" s="76">
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
         <v>100</v>
       </c>
-      <c r="P27" s="43">
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
         <v>0</v>
       </c>
       <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="U27">
         <v>5</v>
       </c>
-      <c r="T27">
+      <c r="V27">
         <v>5</v>
       </c>
-      <c r="U27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -3736,31 +3801,40 @@
         <v>1</v>
       </c>
       <c r="L28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
-      <c r="O28" s="43">
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
         <v>100</v>
       </c>
-      <c r="P28" s="43">
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
         <v>0</v>
       </c>
       <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="U28">
         <v>6</v>
       </c>
-      <c r="T28">
+      <c r="V28">
         <v>6</v>
       </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
@@ -3772,17 +3846,17 @@
       </c>
       <c r="O29" s="43"/>
       <c r="P29" s="43"/>
-      <c r="S29">
+      <c r="U29">
         <v>7</v>
       </c>
-      <c r="T29">
+      <c r="V29">
         <v>7</v>
       </c>
-      <c r="U29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>8</v>
       </c>
@@ -3793,17 +3867,17 @@
         <v>3</v>
       </c>
       <c r="P30" s="43"/>
-      <c r="S30">
+      <c r="U30">
         <v>8</v>
       </c>
-      <c r="T30">
+      <c r="V30">
         <v>8</v>
       </c>
-      <c r="U30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>9</v>
       </c>
@@ -3814,17 +3888,17 @@
         <v>3</v>
       </c>
       <c r="P31" s="43"/>
-      <c r="S31">
+      <c r="U31">
         <v>9</v>
       </c>
-      <c r="T31">
+      <c r="V31">
         <v>9</v>
       </c>
-      <c r="U31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10</v>
       </c>
@@ -3834,17 +3908,17 @@
       <c r="C32">
         <v>4</v>
       </c>
-      <c r="S32">
+      <c r="U32">
         <v>10</v>
       </c>
-      <c r="T32">
+      <c r="V32">
         <v>10</v>
       </c>
-      <c r="U32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>11</v>
       </c>
@@ -3854,17 +3928,17 @@
       <c r="C33">
         <v>4</v>
       </c>
-      <c r="S33">
+      <c r="U33">
         <v>11</v>
       </c>
-      <c r="T33">
+      <c r="V33">
         <v>11</v>
       </c>
-      <c r="U33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>12</v>
       </c>
@@ -3874,17 +3948,17 @@
       <c r="C34">
         <v>4</v>
       </c>
-      <c r="S34">
+      <c r="U34">
         <v>12</v>
       </c>
-      <c r="T34">
+      <c r="V34">
         <v>12</v>
       </c>
-      <c r="U34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
@@ -3895,7 +3969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
@@ -3906,7 +3980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3</v>
       </c>
@@ -3917,7 +3991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3928,29 +4002,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="J43" t="s">
-        <v>115</v>
-      </c>
-      <c r="S43" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="U43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -3973,37 +4047,46 @@
         <v>49</v>
       </c>
       <c r="J44" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="K44" t="s">
         <v>50</v>
       </c>
       <c r="L44" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="M44" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="N44" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="O44" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="P44" t="s">
-        <v>55</v>
+        <v>120</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>121</v>
+      </c>
+      <c r="R44" t="s">
+        <v>122</v>
       </c>
       <c r="S44" t="s">
-        <v>117</v>
-      </c>
-      <c r="T44" t="s">
+        <v>123</v>
+      </c>
+      <c r="U44" t="s">
+        <v>112</v>
+      </c>
+      <c r="V44" t="s">
         <v>48</v>
       </c>
-      <c r="U44" t="s">
+      <c r="W44" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
@@ -4032,10 +4115,10 @@
         <v>12</v>
       </c>
       <c r="L45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M45">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N45">
         <v>0</v>
@@ -4046,17 +4129,26 @@
       <c r="P45">
         <v>0</v>
       </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
       <c r="S45">
-        <v>1</v>
-      </c>
-      <c r="T45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V45">
+        <v>1</v>
+      </c>
+      <c r="W45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -4085,10 +4177,10 @@
         <v>14</v>
       </c>
       <c r="L46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M46">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -4099,17 +4191,26 @@
       <c r="P46">
         <v>0</v>
       </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
       <c r="S46">
-        <v>2</v>
-      </c>
-      <c r="T46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="V46">
+        <v>2</v>
+      </c>
+      <c r="W46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>3</v>
       </c>
@@ -4126,31 +4227,40 @@
         <v>2</v>
       </c>
       <c r="L47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M47">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
         <v>10</v>
       </c>
-      <c r="O47">
+      <c r="P47">
         <v>100</v>
       </c>
-      <c r="P47">
+      <c r="Q47">
         <v>0.5</v>
       </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
       <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="U47">
         <v>3</v>
       </c>
-      <c r="T47">
+      <c r="V47">
         <v>3</v>
       </c>
-      <c r="U47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>4</v>
       </c>
@@ -4160,17 +4270,17 @@
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="S48">
+      <c r="U48">
         <v>4</v>
       </c>
-      <c r="T48">
+      <c r="V48">
         <v>4</v>
       </c>
-      <c r="U48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>5</v>
       </c>
@@ -4180,17 +4290,17 @@
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="S49">
+      <c r="U49">
         <v>5</v>
       </c>
-      <c r="T49">
+      <c r="V49">
         <v>5</v>
       </c>
-      <c r="U49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>6</v>
       </c>
@@ -4200,17 +4310,17 @@
       <c r="C50">
         <v>1</v>
       </c>
-      <c r="S50">
+      <c r="U50">
         <v>6</v>
       </c>
-      <c r="T50">
+      <c r="V50">
         <v>6</v>
       </c>
-      <c r="U50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>7</v>
       </c>
@@ -4220,17 +4330,17 @@
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="S51">
+      <c r="U51">
         <v>7</v>
       </c>
-      <c r="T51">
+      <c r="V51">
         <v>7</v>
       </c>
-      <c r="U51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>8</v>
       </c>
@@ -4240,17 +4350,17 @@
       <c r="C52">
         <v>1</v>
       </c>
-      <c r="S52">
+      <c r="U52">
         <v>8</v>
       </c>
-      <c r="T52">
+      <c r="V52">
         <v>8</v>
       </c>
-      <c r="U52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>9</v>
       </c>
@@ -4260,17 +4370,17 @@
       <c r="C53">
         <v>1</v>
       </c>
-      <c r="S53">
+      <c r="U53">
         <v>9</v>
       </c>
-      <c r="T53">
+      <c r="V53">
         <v>9</v>
       </c>
-      <c r="U53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>10</v>
       </c>
@@ -4280,17 +4390,17 @@
       <c r="C54">
         <v>1</v>
       </c>
-      <c r="S54">
+      <c r="U54">
         <v>10</v>
       </c>
-      <c r="T54">
+      <c r="V54">
         <v>10</v>
       </c>
-      <c r="U54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>11</v>
       </c>
@@ -4300,17 +4410,17 @@
       <c r="C55">
         <v>1</v>
       </c>
-      <c r="S55">
+      <c r="U55">
         <v>11</v>
       </c>
-      <c r="T55">
+      <c r="V55">
         <v>11</v>
       </c>
-      <c r="U55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>12</v>
       </c>
@@ -4320,39 +4430,39 @@
       <c r="C56">
         <v>1</v>
       </c>
-      <c r="S56">
+      <c r="U56">
         <v>12</v>
       </c>
-      <c r="T56">
+      <c r="V56">
         <v>12</v>
       </c>
-      <c r="U56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E61" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="J61" t="s">
-        <v>115</v>
-      </c>
-      <c r="S61" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="U61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>44</v>
       </c>
@@ -4375,37 +4485,46 @@
         <v>49</v>
       </c>
       <c r="J62" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="K62" t="s">
         <v>50</v>
       </c>
       <c r="L62" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="M62" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="N62" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="O62" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="P62" t="s">
-        <v>55</v>
+        <v>120</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>121</v>
+      </c>
+      <c r="R62" t="s">
+        <v>122</v>
       </c>
       <c r="S62" t="s">
-        <v>117</v>
-      </c>
-      <c r="T62" t="s">
+        <v>123</v>
+      </c>
+      <c r="U62" t="s">
+        <v>112</v>
+      </c>
+      <c r="V62" t="s">
         <v>48</v>
       </c>
-      <c r="U62" t="s">
+      <c r="W62" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1</v>
       </c>
@@ -4434,10 +4553,10 @@
         <v>12</v>
       </c>
       <c r="L63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M63">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N63">
         <v>0</v>
@@ -4448,17 +4567,26 @@
       <c r="P63">
         <v>0</v>
       </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
       <c r="S63">
-        <v>1</v>
-      </c>
-      <c r="T63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="V63">
+        <v>1</v>
+      </c>
+      <c r="W63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2</v>
       </c>
@@ -4484,34 +4612,43 @@
         <v>2</v>
       </c>
       <c r="K64">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="L64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M64">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N64">
         <v>0</v>
       </c>
       <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
         <v>100</v>
       </c>
-      <c r="P64">
+      <c r="Q64">
+        <v>1</v>
+      </c>
+      <c r="R64">
         <v>1</v>
       </c>
       <c r="S64">
-        <v>2</v>
-      </c>
-      <c r="T64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V64">
+        <v>2</v>
+      </c>
+      <c r="W64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3</v>
       </c>
@@ -4525,34 +4662,43 @@
         <v>3</v>
       </c>
       <c r="K65">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="L65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M65">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
         <v>100</v>
       </c>
-      <c r="O65">
+      <c r="P65">
         <v>200</v>
       </c>
-      <c r="P65">
+      <c r="Q65">
         <v>0.5</v>
       </c>
+      <c r="R65">
+        <v>1</v>
+      </c>
       <c r="S65">
+        <v>1</v>
+      </c>
+      <c r="U65">
         <v>3</v>
       </c>
-      <c r="T65">
+      <c r="V65">
         <v>3</v>
       </c>
-      <c r="U65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>4</v>
       </c>
@@ -4562,17 +4708,17 @@
       <c r="C66">
         <v>1</v>
       </c>
-      <c r="S66">
+      <c r="U66">
         <v>4</v>
       </c>
-      <c r="T66">
+      <c r="V66">
         <v>4</v>
       </c>
-      <c r="U66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>5</v>
       </c>
@@ -4582,17 +4728,17 @@
       <c r="C67">
         <v>1</v>
       </c>
-      <c r="S67">
+      <c r="U67">
         <v>5</v>
       </c>
-      <c r="T67">
+      <c r="V67">
         <v>5</v>
       </c>
-      <c r="U67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>6</v>
       </c>
@@ -4602,17 +4748,17 @@
       <c r="C68">
         <v>1</v>
       </c>
-      <c r="S68">
+      <c r="U68">
         <v>6</v>
       </c>
-      <c r="T68">
+      <c r="V68">
         <v>6</v>
       </c>
-      <c r="U68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>7</v>
       </c>
@@ -4622,17 +4768,17 @@
       <c r="C69">
         <v>1</v>
       </c>
-      <c r="S69">
+      <c r="U69">
         <v>7</v>
       </c>
-      <c r="T69">
+      <c r="V69">
         <v>7</v>
       </c>
-      <c r="U69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>8</v>
       </c>
@@ -4642,17 +4788,17 @@
       <c r="C70">
         <v>1</v>
       </c>
-      <c r="S70">
+      <c r="U70">
         <v>8</v>
       </c>
-      <c r="T70">
+      <c r="V70">
         <v>8</v>
       </c>
-      <c r="U70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>9</v>
       </c>
@@ -4662,17 +4808,17 @@
       <c r="C71">
         <v>1</v>
       </c>
-      <c r="S71">
+      <c r="U71">
         <v>9</v>
       </c>
-      <c r="T71">
+      <c r="V71">
         <v>9</v>
       </c>
-      <c r="U71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>10</v>
       </c>
@@ -4682,17 +4828,17 @@
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="S72">
+      <c r="U72">
         <v>10</v>
       </c>
-      <c r="T72">
+      <c r="V72">
         <v>10</v>
       </c>
-      <c r="U72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>11</v>
       </c>
@@ -4702,17 +4848,17 @@
       <c r="C73">
         <v>1</v>
       </c>
-      <c r="S73">
+      <c r="U73">
         <v>11</v>
       </c>
-      <c r="T73">
+      <c r="V73">
         <v>11</v>
       </c>
-      <c r="U73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>12</v>
       </c>
@@ -4722,13 +4868,13 @@
       <c r="C74">
         <v>1</v>
       </c>
-      <c r="S74">
+      <c r="U74">
         <v>12</v>
       </c>
-      <c r="T74">
+      <c r="V74">
         <v>12</v>
       </c>
-      <c r="U74">
+      <c r="W74">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated for calcrule24 correction
</commit_message>
<xml_diff>
--- a/ftest/data/fm23/worked_example_policy_calculation_locfac_catxol_reinsurance.xlsx
+++ b/ftest/data/fm23/worked_example_policy_calculation_locfac_catxol_reinsurance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B9502424-6FD3-45A5-AA77-746CDD9B3603}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6D4EEF2B-5717-443F-A8B7-FD0B77AF8344}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -823,6 +823,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -848,27 +869,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1604,26 +1604,26 @@
       <c r="B25" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="64">
+      <c r="C25" s="71">
         <v>100</v>
       </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="64">
+      <c r="D25" s="71"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="71">
         <v>100</v>
       </c>
-      <c r="G25" s="64"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="66">
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73">
         <v>100</v>
       </c>
-      <c r="J25" s="64"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="64">
+      <c r="J25" s="71"/>
+      <c r="K25" s="72"/>
+      <c r="L25" s="71">
         <v>100</v>
       </c>
-      <c r="M25" s="64"/>
-      <c r="N25" s="65"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="72"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="11"/>
@@ -1864,30 +1864,30 @@
       <c r="B34" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="67">
+      <c r="C34" s="74">
         <f>SUMIF($C$21:$N$21,C21,$C$31:$N$31)</f>
         <v>1600</v>
       </c>
-      <c r="D34" s="67"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="67">
+      <c r="D34" s="74"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="74">
         <f>SUMIF($C$21:$N$21,F21,$C$31:$N$31)</f>
         <v>1600</v>
       </c>
-      <c r="G34" s="67"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="67">
+      <c r="G34" s="74"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="74">
         <f>SUMIF($C$21:$N$21,I21,$C$31:$N$31)</f>
         <v>1600</v>
       </c>
-      <c r="J34" s="67"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="67">
+      <c r="J34" s="74"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="74">
         <f>SUMIF($C$21:$N$21,L21,$C$31:$N$31)</f>
         <v>1600</v>
       </c>
-      <c r="M34" s="67"/>
-      <c r="N34" s="68"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="75"/>
       <c r="O34" s="8"/>
       <c r="P34" s="24"/>
       <c r="Q34" s="11"/>
@@ -1899,30 +1899,30 @@
       <c r="B35" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="60">
+      <c r="C35" s="67">
         <f>MIN(C34, C25)</f>
         <v>100</v>
       </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="60">
+      <c r="D35" s="68"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="67">
         <f>MIN(F34, F25)</f>
         <v>100</v>
       </c>
-      <c r="G35" s="61"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="60">
+      <c r="G35" s="68"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="67">
         <f>MIN(I34, I25)</f>
         <v>100</v>
       </c>
-      <c r="J35" s="61"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="63">
+      <c r="J35" s="68"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="70">
         <f>MIN(L34, L25)</f>
         <v>100</v>
       </c>
-      <c r="M35" s="61"/>
-      <c r="N35" s="62"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="69"/>
       <c r="O35" s="12">
         <f>SUM(C35:N35)</f>
         <v>400</v>
@@ -2252,11 +2252,11 @@
       <c r="A53" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="69">
-        <v>1</v>
-      </c>
-      <c r="D53" s="69"/>
-      <c r="E53" s="70"/>
+      <c r="C53" s="60">
+        <v>1</v>
+      </c>
+      <c r="D53" s="60"/>
+      <c r="E53" s="61"/>
       <c r="H53" s="41"/>
       <c r="N53" s="41"/>
     </row>
@@ -2264,11 +2264,11 @@
       <c r="A54" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="69" t="s">
+      <c r="C54" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="69"/>
-      <c r="E54" s="70"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="61"/>
       <c r="H54" s="41"/>
       <c r="N54" s="41"/>
     </row>
@@ -2276,11 +2276,11 @@
       <c r="A55" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="69">
-        <v>1</v>
-      </c>
-      <c r="D55" s="69"/>
-      <c r="E55" s="70"/>
+      <c r="C55" s="60">
+        <v>1</v>
+      </c>
+      <c r="D55" s="60"/>
+      <c r="E55" s="61"/>
       <c r="H55" s="41"/>
       <c r="N55" s="41"/>
     </row>
@@ -2288,11 +2288,11 @@
       <c r="A56" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="73">
+      <c r="C56" s="64">
         <v>10</v>
       </c>
-      <c r="D56" s="73"/>
-      <c r="E56" s="70"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="61"/>
       <c r="H56" s="41"/>
       <c r="N56" s="41"/>
     </row>
@@ -2300,12 +2300,12 @@
       <c r="A57" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C57" s="73">
+      <c r="C57" s="64">
         <f>MAX(0, SUM(C50:E50)-C56)</f>
         <v>90</v>
       </c>
-      <c r="D57" s="73"/>
-      <c r="E57" s="70"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="61"/>
       <c r="H57" s="41"/>
       <c r="N57" s="41"/>
     </row>
@@ -2313,11 +2313,11 @@
       <c r="A58" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="73">
+      <c r="C58" s="64">
         <v>100</v>
       </c>
-      <c r="D58" s="73"/>
-      <c r="E58" s="70"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="61"/>
       <c r="H58" s="41"/>
       <c r="N58" s="41"/>
     </row>
@@ -2325,12 +2325,12 @@
       <c r="A59" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C59" s="73">
+      <c r="C59" s="64">
         <f>IF(C58="Unlimited", C57, MIN(C57, C58))</f>
         <v>90</v>
       </c>
-      <c r="D59" s="73"/>
-      <c r="E59" s="70"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="61"/>
       <c r="H59" s="41"/>
       <c r="N59" s="41"/>
     </row>
@@ -2338,11 +2338,11 @@
       <c r="A60" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C60" s="74">
+      <c r="C60" s="65">
         <v>0.5</v>
       </c>
-      <c r="D60" s="74"/>
-      <c r="E60" s="75"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="66"/>
       <c r="H60" s="41"/>
       <c r="N60" s="41"/>
     </row>
@@ -2350,12 +2350,12 @@
       <c r="A61" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="73">
+      <c r="C61" s="64">
         <f>C60*C59</f>
         <v>45</v>
       </c>
-      <c r="D61" s="73"/>
-      <c r="E61" s="70"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="61"/>
       <c r="H61" s="41"/>
       <c r="N61" s="41"/>
     </row>
@@ -2363,9 +2363,9 @@
       <c r="A62" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="71"/>
-      <c r="D62" s="71"/>
-      <c r="E62" s="72"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="62"/>
+      <c r="E62" s="63"/>
       <c r="H62" s="41"/>
       <c r="N62" s="41"/>
     </row>
@@ -2373,9 +2373,9 @@
       <c r="A63" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C63" s="71"/>
-      <c r="D63" s="71"/>
-      <c r="E63" s="72"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="62"/>
+      <c r="E63" s="63"/>
       <c r="H63" s="41"/>
       <c r="N63" s="41"/>
     </row>
@@ -2383,12 +2383,12 @@
       <c r="A64" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="73">
+      <c r="C64" s="64">
         <f>MIN(C61,IF(OR(C63="Unlimited",C63=""),10^18,C63))</f>
         <v>45</v>
       </c>
-      <c r="D64" s="73"/>
-      <c r="E64" s="70"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="61"/>
       <c r="H64" s="41"/>
       <c r="N64" s="41"/>
     </row>
@@ -2848,6 +2848,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
     <mergeCell ref="C54:E54"/>
     <mergeCell ref="C53:E53"/>
     <mergeCell ref="C63:E63"/>
@@ -2860,18 +2872,6 @@
     <mergeCell ref="C57:E57"/>
     <mergeCell ref="C59:E59"/>
     <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -2889,8 +2889,8 @@
   </sheetPr>
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L67" sqref="L67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R66" sqref="R66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4680,10 +4680,10 @@
         <v>200</v>
       </c>
       <c r="Q65">
+        <v>1</v>
+      </c>
+      <c r="R65">
         <v>0.5</v>
-      </c>
-      <c r="R65">
-        <v>1</v>
       </c>
       <c r="S65">
         <v>1</v>

</xml_diff>